<commit_message>
fix array data en archivos para generar la tabla detalle
</commit_message>
<xml_diff>
--- a/detalle.xlsx
+++ b/detalle.xlsx
@@ -13,6 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Lineal" sheetId="1" r:id="rId1"/>
+    <sheet name="Parabola" sheetId="2" r:id="rId2"/>
+    <sheet name="Potencial" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="22">
   <si>
     <t>X</t>
   </si>
@@ -48,6 +50,48 @@
   </si>
   <si>
     <t>Eyx</t>
+  </si>
+  <si>
+    <t>X^3</t>
+  </si>
+  <si>
+    <t>X^4</t>
+  </si>
+  <si>
+    <t>X^2*Y</t>
+  </si>
+  <si>
+    <t>Ex^3</t>
+  </si>
+  <si>
+    <t>Ex^4</t>
+  </si>
+  <si>
+    <t>Ex^2*y</t>
+  </si>
+  <si>
+    <t>X=ln(x)</t>
+  </si>
+  <si>
+    <t>Y=ln(y)</t>
+  </si>
+  <si>
+    <t>X^2=ln(x)^2</t>
+  </si>
+  <si>
+    <t>X*Y=ln(x)ln(y)</t>
+  </si>
+  <si>
+    <t>EX</t>
+  </si>
+  <si>
+    <t>EY</t>
+  </si>
+  <si>
+    <t>EX^2</t>
+  </si>
+  <si>
+    <t>EXY</t>
   </si>
 </sst>
 </file>
@@ -466,7 +510,7 @@
         <v>90</v>
       </c>
       <c r="D7" t="n">
-        <v>90</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -500,4 +544,460 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.728</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.0736</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>6.48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5.832</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10.4976</v>
+      </c>
+      <c r="F3" t="n">
+        <v>10.62</v>
+      </c>
+      <c r="G3" t="n">
+        <v>19.116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9.61</v>
+      </c>
+      <c r="D4" t="n">
+        <v>29.791</v>
+      </c>
+      <c r="E4" t="n">
+        <v>92.3521</v>
+      </c>
+      <c r="F4" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="G4" t="n">
+        <v>67.27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="B5" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>24.01</v>
+      </c>
+      <c r="D5" t="n">
+        <v>117.649</v>
+      </c>
+      <c r="E5" t="n">
+        <v>576.4801</v>
+      </c>
+      <c r="F5" t="n">
+        <v>38.22</v>
+      </c>
+      <c r="G5" t="n">
+        <v>187.278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="B6" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>32.49</v>
+      </c>
+      <c r="D6" t="n">
+        <v>185.193</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1055.6001</v>
+      </c>
+      <c r="F6" t="n">
+        <v>41.04</v>
+      </c>
+      <c r="G6" t="n">
+        <v>233.928</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="C7" t="n">
+        <v>50.41</v>
+      </c>
+      <c r="D7" t="n">
+        <v>357.911</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2541.1681</v>
+      </c>
+      <c r="F7" t="n">
+        <v>48.28</v>
+      </c>
+      <c r="G7" t="n">
+        <v>342.788</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>73.96</v>
+      </c>
+      <c r="D8" t="n">
+        <v>636.056</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5470.0816</v>
+      </c>
+      <c r="F8" t="n">
+        <v>38.7</v>
+      </c>
+      <c r="G8" t="n">
+        <v>332.82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="n">
+        <v>9.8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>96.04</v>
+      </c>
+      <c r="D9" t="n">
+        <v>941.192</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9223.6816</v>
+      </c>
+      <c r="F9" t="n">
+        <v>26.46</v>
+      </c>
+      <c r="G9" t="n">
+        <v>259.308</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="n">
+        <v>42.2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>46.4</v>
+      </c>
+      <c r="C10" t="n">
+        <v>291.2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2275.352</v>
+      </c>
+      <c r="E10" t="n">
+        <v>18971.9348</v>
+      </c>
+      <c r="F10" t="n">
+        <v>230.42</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1448.988</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="n">
+        <v>42.2</v>
+      </c>
+      <c r="B12" t="n">
+        <v>46.4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>291.2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2275.352</v>
+      </c>
+      <c r="E12" t="n">
+        <v>18971.9348</v>
+      </c>
+      <c r="F12" t="n">
+        <v>230.42</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1448.988</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.8" bottom="0.8" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>-0.916290731874155</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="n">
+        <v>0.693147180559945</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-0.356674943938732</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.480453013918201</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.247228231767509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="n">
+        <v>0.916290731874155</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-0.22314355131421</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.839588705318475</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.204464367946695</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="n">
+        <v>1.38629436111989</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.92181205567281</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="n">
+        <v>1.79175946922805</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.182321556793955</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3.2104019955684</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.326676375829969</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="n">
+        <v>2.07944154167984</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.262364264467491</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4.32407712526381</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.545571150585976</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="n">
+        <v>2.14006616349627</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.336472236621213</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4.57988318414165</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.720072848548968</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="n">
+        <v>9.00699944795815</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.714951169244439</v>
+      </c>
+      <c r="C9" t="n">
+        <v>15.3562160798833</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.14062777525071</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="n">
+        <v>9.00699944795815</v>
+      </c>
+      <c r="B11" t="n">
+        <v>-0.714951169244439</v>
+      </c>
+      <c r="C11" t="n">
+        <v>15.3562160798833</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.14062777525071</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.8" bottom="0.8" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Seleccion de archivo output para mostrar detalles
</commit_message>
<xml_diff>
--- a/detalle.xlsx
+++ b/detalle.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manu\Documents\GitHub\mat-sup-tp-2c-2017-minimos-cuadrados\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="6936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lineal" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,12 +408,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -547,14 +549,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,214 +579,214 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="n">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1.2</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>4.5</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>1.44</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>1.728</v>
       </c>
-      <c r="E2" t="n">
-        <v>2.0736</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="E2">
+        <v>2.0735999999999999</v>
+      </c>
+      <c r="F2">
         <v>5.4</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>6.48</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="n">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>1.8</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>5.9</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>3.24</v>
       </c>
-      <c r="D3" t="n">
-        <v>5.832</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="D3">
+        <v>5.8319999999999999</v>
+      </c>
+      <c r="E3">
         <v>10.4976</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>10.62</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>19.116</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="n">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3.1</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>7</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>9.61</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>29.791</v>
       </c>
-      <c r="E4" t="n">
-        <v>92.3521</v>
-      </c>
-      <c r="F4" t="n">
+      <c r="E4">
+        <v>92.352099999999993</v>
+      </c>
+      <c r="F4">
         <v>21.7</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>67.27</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="B5" t="n">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B5">
         <v>7.8</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>24.01</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>117.649</v>
       </c>
-      <c r="E5" t="n">
-        <v>576.4801</v>
-      </c>
-      <c r="F5" t="n">
+      <c r="E5">
+        <v>576.48009999999999</v>
+      </c>
+      <c r="F5">
         <v>38.22</v>
       </c>
-      <c r="G5" t="n">
-        <v>187.278</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="n">
+      <c r="G5">
+        <v>187.27799999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>5.7</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>7.2</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>32.49</v>
       </c>
-      <c r="D6" t="n">
-        <v>185.193</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1055.6001</v>
-      </c>
-      <c r="F6" t="n">
+      <c r="D6">
+        <v>185.19300000000001</v>
+      </c>
+      <c r="E6">
+        <v>1055.6001000000001</v>
+      </c>
+      <c r="F6">
         <v>41.04</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>233.928</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="n">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>7.1</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>6.8</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>50.41</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>357.911</v>
       </c>
-      <c r="E7" t="n">
-        <v>2541.1681</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="E7">
+        <v>2541.1680999999999</v>
+      </c>
+      <c r="F7">
         <v>48.28</v>
       </c>
-      <c r="G7" t="n">
-        <v>342.788</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="n">
+      <c r="G7">
+        <v>342.78800000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>8.6</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>4.5</v>
       </c>
-      <c r="C8" t="n">
-        <v>73.96</v>
-      </c>
-      <c r="D8" t="n">
-        <v>636.056</v>
-      </c>
-      <c r="E8" t="n">
-        <v>5470.0816</v>
-      </c>
-      <c r="F8" t="n">
-        <v>38.7</v>
-      </c>
-      <c r="G8" t="n">
+      <c r="C8">
+        <v>73.959999999999994</v>
+      </c>
+      <c r="D8">
+        <v>636.05600000000004</v>
+      </c>
+      <c r="E8">
+        <v>5470.0816000000004</v>
+      </c>
+      <c r="F8">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="G8">
         <v>332.82</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="n">
-        <v>9.8</v>
-      </c>
-      <c r="B9" t="n">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="B9">
         <v>2.7</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>96.04</v>
       </c>
-      <c r="D9" t="n">
-        <v>941.192</v>
-      </c>
-      <c r="E9" t="n">
-        <v>9223.6816</v>
-      </c>
-      <c r="F9" t="n">
+      <c r="D9">
+        <v>941.19200000000001</v>
+      </c>
+      <c r="E9">
+        <v>9223.6815999999999</v>
+      </c>
+      <c r="F9">
         <v>26.46</v>
       </c>
-      <c r="G9" t="n">
-        <v>259.308</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="n">
+      <c r="G9">
+        <v>259.30799999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>42.2</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>46.4</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>291.2</v>
       </c>
-      <c r="D10" t="n">
-        <v>2275.352</v>
-      </c>
-      <c r="E10" t="n">
-        <v>18971.9348</v>
-      </c>
-      <c r="F10" t="n">
+      <c r="D10">
+        <v>2275.3519999999999</v>
+      </c>
+      <c r="E10">
+        <v>18971.934799999999</v>
+      </c>
+      <c r="F10">
         <v>230.42</v>
       </c>
-      <c r="G10" t="n">
-        <v>1448.988</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="G10">
+        <v>1448.9880000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -807,27 +809,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="n">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>42.2</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>46.4</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>291.2</v>
       </c>
-      <c r="D12" t="n">
-        <v>2275.352</v>
-      </c>
-      <c r="E12" t="n">
-        <v>18971.9348</v>
-      </c>
-      <c r="F12" t="n">
+      <c r="D12">
+        <v>2275.3519999999999</v>
+      </c>
+      <c r="E12">
+        <v>18971.934799999999</v>
+      </c>
+      <c r="F12">
         <v>230.42</v>
       </c>
-      <c r="G12" t="n">
-        <v>1448.988</v>
+      <c r="G12">
+        <v>1448.9880000000001</v>
       </c>
     </row>
   </sheetData>
@@ -836,14 +838,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -857,119 +859,119 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="n">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>-0.916290731874155</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
-        <v>-0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="n">
-        <v>0.693147180559945</v>
-      </c>
-      <c r="B3" t="n">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.69314718055994495</v>
+      </c>
+      <c r="B3">
         <v>-0.356674943938732</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>0.480453013918201</v>
       </c>
-      <c r="D3" t="n">
-        <v>-0.247228231767509</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="n">
+      <c r="D3">
+        <v>-0.24722823176750899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>0.916290731874155</v>
       </c>
-      <c r="B4" t="n">
-        <v>-0.22314355131421</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.839588705318475</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.204464367946695</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="n">
-        <v>1.38629436111989</v>
-      </c>
-      <c r="B5" t="n">
+      <c r="B4">
+        <v>-0.22314355131420999</v>
+      </c>
+      <c r="C4">
+        <v>0.83958870531847496</v>
+      </c>
+      <c r="D4">
+        <v>-0.20446436794669501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1.3862943611198899</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>1.92181205567281</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="n">
-        <v>1.79175946922805</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.182321556793955</v>
-      </c>
-      <c r="C6" t="n">
-        <v>3.2104019955684</v>
-      </c>
-      <c r="D6" t="n">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1.7917594692280501</v>
+      </c>
+      <c r="B6">
+        <v>0.18232155679395501</v>
+      </c>
+      <c r="C6">
+        <v>3.2104019955683998</v>
+      </c>
+      <c r="D6">
         <v>0.326676375829969</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="n">
-        <v>2.07944154167984</v>
-      </c>
-      <c r="B7" t="n">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2.0794415416798402</v>
+      </c>
+      <c r="B7">
         <v>0.262364264467491</v>
       </c>
-      <c r="C7" t="n">
-        <v>4.32407712526381</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.545571150585976</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="n">
-        <v>2.14006616349627</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.336472236621213</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4.57988318414165</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.720072848548968</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="n">
-        <v>9.00699944795815</v>
-      </c>
-      <c r="B9" t="n">
-        <v>-0.714951169244439</v>
-      </c>
-      <c r="C9" t="n">
+      <c r="C7">
+        <v>4.3240771252638099</v>
+      </c>
+      <c r="D7">
+        <v>0.54557115058597605</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2.1400661634962699</v>
+      </c>
+      <c r="B8">
+        <v>0.33647223662121301</v>
+      </c>
+      <c r="C8">
+        <v>4.5798831841416501</v>
+      </c>
+      <c r="D8">
+        <v>0.72007284854896803</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9.0069994479581492</v>
+      </c>
+      <c r="B9">
+        <v>-0.71495116924443902</v>
+      </c>
+      <c r="C9">
         <v>15.3562160798833</v>
       </c>
-      <c r="D9" t="n">
-        <v>1.14062777525071</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9">
+        <v>1.1406277752507099</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -983,18 +985,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="n">
-        <v>9.00699944795815</v>
-      </c>
-      <c r="B11" t="n">
-        <v>-0.714951169244439</v>
-      </c>
-      <c r="C11" t="n">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9.0069994479581492</v>
+      </c>
+      <c r="B11">
+        <v>-0.71495116924443902</v>
+      </c>
+      <c r="C11">
         <v>15.3562160798833</v>
       </c>
-      <c r="D11" t="n">
-        <v>1.14062777525071</v>
+      <c r="D11">
+        <v>1.1406277752507099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tabla de comparaciones. V.1.1
</commit_message>
<xml_diff>
--- a/detalle.xlsx
+++ b/detalle.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="6936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="6936" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lineal" sheetId="1" r:id="rId1"/>
     <sheet name="Parabola" sheetId="2" r:id="rId2"/>
     <sheet name="Potencial" sheetId="3" r:id="rId3"/>
+    <sheet name="Comparacion" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="37">
   <si>
     <t>X</t>
   </si>
@@ -92,6 +93,51 @@
   </si>
   <si>
     <t>EXY</t>
+  </si>
+  <si>
+    <t>DATOS</t>
+  </si>
+  <si>
+    <t>Indice</t>
+  </si>
+  <si>
+    <t>Xi</t>
+  </si>
+  <si>
+    <t>Yi</t>
+  </si>
+  <si>
+    <t>Mod 1 :Lineal</t>
+  </si>
+  <si>
+    <t>Mod 2 :Cuadratico</t>
+  </si>
+  <si>
+    <t>Mod 3 :Exponencial</t>
+  </si>
+  <si>
+    <t>Mod 4 :Potencial</t>
+  </si>
+  <si>
+    <t>Mod 5: Hiperbolico</t>
+  </si>
+  <si>
+    <t>Error Modelo 1</t>
+  </si>
+  <si>
+    <t>Error Modelo 2</t>
+  </si>
+  <si>
+    <t>Error Modelo 3</t>
+  </si>
+  <si>
+    <t>Error Modelo 4</t>
+  </si>
+  <si>
+    <t>Error Modelo 5</t>
+  </si>
+  <si>
+    <t>Modelos aproximantes</t>
   </si>
 </sst>
 </file>
@@ -411,13 +457,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,91 +477,91 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="n">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>4</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="n">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>9</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>16</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="n">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>12</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>25</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="n">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>18</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>36</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="n">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>20</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>45</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>90</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -529,17 +575,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="n">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>20</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>45</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>90</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>220</v>
       </c>
     </row>
@@ -1002,4 +1048,168 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.8" bottom="0.8" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-8.286</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.742</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-21.572</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>8</v>
+      </c>
+      <c r="D5" t="n">
+        <v>9</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-40.858</v>
+      </c>
+      <c r="F5" t="n">
+        <v>6.366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>12</v>
+      </c>
+      <c r="D6" t="n">
+        <v>13</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-66.144</v>
+      </c>
+      <c r="F6" t="n">
+        <v>12.17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>18</v>
+      </c>
+      <c r="D7" t="n">
+        <v>17</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-97.43</v>
+      </c>
+      <c r="F7" t="n">
+        <v>23.266</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.8" bottom="0.8" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tabla de comparacion pulida
</commit_message>
<xml_diff>
--- a/detalle.xlsx
+++ b/detalle.xlsx
@@ -1165,7 +1165,7 @@
         <v>2.05524627</v>
       </c>
       <c r="E3" t="n">
-        <v>0.25381794</v>
+        <v>3.7322535</v>
       </c>
       <c r="F3" t="n">
         <v>3.01303709</v>
@@ -1174,13 +1174,13 @@
         <v>2.38344367</v>
       </c>
       <c r="H3" t="n">
-        <v>0.66143869</v>
+        <v>3.35198412</v>
       </c>
       <c r="I3" t="n">
         <v>13.87209398</v>
       </c>
       <c r="J3" t="n">
-        <v>69715.93342805</v>
+        <v>1.64153286</v>
       </c>
       <c r="K3" t="n">
         <v>5.4483892</v>
@@ -1189,7 +1189,7 @@
         <v>44.16280073</v>
       </c>
       <c r="M3" t="n">
-        <v>572.56168999</v>
+        <v>0.07530045</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1206,7 +1206,7 @@
         <v>2.8385131</v>
       </c>
       <c r="E4" t="n">
-        <v>1.78390513</v>
+        <v>3.57582647</v>
       </c>
       <c r="F4" t="n">
         <v>3.39529779</v>
@@ -1215,7 +1215,7 @@
         <v>4.19103767</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6163901</v>
+        <v>3.59696234</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1232,7 +1232,7 @@
         <v>3.49123546</v>
       </c>
       <c r="E5" t="n">
-        <v>5.13618861</v>
+        <v>3.59021725</v>
       </c>
       <c r="F5" t="n">
         <v>3.75064273</v>
@@ -1241,7 +1241,7 @@
         <v>4.90022798</v>
       </c>
       <c r="H5" t="n">
-        <v>0.57884961</v>
+        <v>3.83023835</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1258,7 +1258,7 @@
         <v>5.05776913</v>
       </c>
       <c r="E6" t="n">
-        <v>20.8862328</v>
+        <v>4.16163355</v>
       </c>
       <c r="F6" t="n">
         <v>4.76269184</v>
@@ -1267,7 +1267,7 @@
         <v>5.99140402</v>
       </c>
       <c r="H6" t="n">
-        <v>0.48875244</v>
+        <v>4.53630881</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1284,7 +1284,7 @@
         <v>5.71049149</v>
       </c>
       <c r="E7" t="n">
-        <v>30.65898613</v>
+        <v>4.62342302</v>
       </c>
       <c r="F7" t="n">
         <v>5.26114545</v>
@@ -1293,7 +1293,7 @@
         <v>6.32945745</v>
       </c>
       <c r="H7" t="n">
-        <v>0.45121195</v>
+        <v>4.91372624</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1310,7 +1310,7 @@
         <v>6.49375832</v>
       </c>
       <c r="E8" t="n">
-        <v>44.87894314</v>
+        <v>5.35126635</v>
       </c>
       <c r="F8" t="n">
         <v>5.92862118</v>
@@ -1319,7 +1319,7 @@
         <v>6.68427784</v>
       </c>
       <c r="H8" t="n">
-        <v>0.40616336</v>
+        <v>5.45871984</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1336,7 +1336,7 @@
         <v>7.27702515</v>
       </c>
       <c r="E9" t="n">
-        <v>61.81815796</v>
+        <v>6.26859618</v>
       </c>
       <c r="F9" t="n">
         <v>6.68077882</v>
@@ -1345,7 +1345,7 @@
         <v>6.99818129</v>
       </c>
       <c r="H9" t="n">
-        <v>0.36111477</v>
+        <v>6.13968788</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1362,7 +1362,7 @@
         <v>7.66865857</v>
       </c>
       <c r="E10" t="n">
-        <v>71.30748705</v>
+        <v>6.79831853</v>
       </c>
       <c r="F10" t="n">
         <v>7.09191938</v>
@@ -1371,7 +1371,7 @@
         <v>7.14299809</v>
       </c>
       <c r="H10" t="n">
-        <v>0.33859048</v>
+        <v>6.54812268</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1388,7 +1388,7 @@
         <v>8.4519254</v>
       </c>
       <c r="E11" t="n">
-        <v>92.3255886</v>
+        <v>7.99987812</v>
       </c>
       <c r="F11" t="n">
         <v>7.99166337</v>
@@ -1397,7 +1397,7 @@
         <v>7.41281346</v>
       </c>
       <c r="H11" t="n">
-        <v>0.29354189</v>
+        <v>7.55303439</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1414,7 +1414,7 @@
         <v>9.49628118</v>
       </c>
       <c r="E12" t="n">
-        <v>124.5796806</v>
+        <v>9.89671435</v>
       </c>
       <c r="F12" t="n">
         <v>9.37134023</v>
@@ -1423,7 +1423,7 @@
         <v>7.73889234</v>
       </c>
       <c r="H12" t="n">
-        <v>0.23347711</v>
+        <v>9.49614301</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1440,7 +1440,7 @@
         <v>10.01845906</v>
       </c>
       <c r="E13" t="n">
-        <v>142.51956515</v>
+        <v>10.9714568</v>
       </c>
       <c r="F13" t="n">
         <v>10.14808198</v>
@@ -1449,7 +1449,7 @@
         <v>7.89004695</v>
       </c>
       <c r="H13" t="n">
-        <v>0.20344471</v>
+        <v>10.89795819</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1466,7 +1466,7 @@
         <v>10.54063695</v>
       </c>
       <c r="E14" t="n">
-        <v>161.66800873</v>
+        <v>12.13041548</v>
       </c>
       <c r="F14" t="n">
         <v>10.98920382</v>
@@ -1475,7 +1475,7 @@
         <v>8.03442808</v>
       </c>
       <c r="H14" t="n">
-        <v>0.17341232</v>
+        <v>12.78531975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>